<commit_message>
Results for first report draft.  Updated costs to $2021.  Added TMD damper sensitivity
</commit_message>
<xml_diff>
--- a/data/NASA Floater CAPEX Estimates 031522.xlsx
+++ b/data/NASA Floater CAPEX Estimates 031522.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\NASA Floater\LCOE analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC05481-8614-44EA-938D-8DB18491D187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CB6618-C504-415D-8811-125B96555AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ED2218FA-9BBC-49B1-AFB3-38C65EBAFD2A}"/>
   </bookViews>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Material Cost/Hull</t>
   </si>
@@ -293,9 +292,6 @@
     <t>TOTAL PLATFORM CAPEX ($)</t>
   </si>
   <si>
-    <t>*2018 US Dollars</t>
-  </si>
-  <si>
     <t>Turbine Rating (kW)</t>
   </si>
   <si>
@@ -321,6 +317,21 @@
   </si>
   <si>
     <t>Inflated using BLS CPI from 1/1/2018 to 1/1/2021(https://www.bls.gov/data/inflation_calculator.htm)</t>
+  </si>
+  <si>
+    <t>Comparison cases</t>
+  </si>
+  <si>
+    <t>AQUA VENTUS PLATFORM CAPEX ($/KW)</t>
+  </si>
+  <si>
+    <t>TMD sensitivity ($)</t>
+  </si>
+  <si>
+    <t>CPI ratio</t>
+  </si>
+  <si>
+    <t>TMD sclae</t>
   </si>
 </sst>
 </file>
@@ -798,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F63F25-6DA0-414B-BEA5-874ACB5A3706}">
-  <dimension ref="A2:Z14"/>
+  <dimension ref="A2:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,7 +825,7 @@
   <sheetData>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="15">
         <v>15000</v>
@@ -831,7 +842,7 @@
         <v>7089349.3494419996</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
         <v>0</v>
@@ -845,13 +856,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="15">
         <v>1.2</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P4" t="s">
         <v>2</v>
@@ -866,12 +877,16 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="16">
         <f>B4*B3</f>
         <v>8507219.2193303984</v>
       </c>
+      <c r="F5">
+        <f>22200000/15000</f>
+        <v>1480</v>
+      </c>
       <c r="P5" t="s">
         <v>3</v>
       </c>
@@ -883,6 +898,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B6" s="16"/>
       <c r="P6" t="s">
         <v>4</v>
       </c>
@@ -926,42 +942,103 @@
       </c>
       <c r="Z10" s="1"/>
     </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1"/>
+    </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="17">
+        <f>B10*B11</f>
+        <v>214769.86249999999</v>
+      </c>
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="19">
-        <f>B9+B10</f>
+      <c r="B14" s="19">
+        <f>B9+B12</f>
         <v>5252423.5333419824</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="17">
-        <f>B12/B2</f>
+      <c r="C14" s="18"/>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <f>369/350</f>
+        <v>1.0542857142857143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="17">
+        <f>B14/B2</f>
         <v>350.16156888946551</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="17">
+        <f>B15*F14</f>
+        <v>369.17033977203647</v>
+      </c>
+      <c r="C16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="17">
-        <v>369.54</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="17">
+        <f>B16*15000</f>
+        <v>5537555.0965805473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="15">
+        <v>690</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="15">
+        <v>728</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -974,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDC703A-9E80-478F-A3E7-EDA79FD124E5}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>